<commit_message>
ReadFile still remain interactable after reading + ending the page change the final button to end button, when onclick closes the readFile
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterKeyEvent.xlsx
+++ b/Assets/Data/Excel/MasterKeyEvent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6D6073-CA88-414D-BF62-7B34340CEA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E1C16D-EA2A-4AD0-B30C-53AFC9BEF952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>id</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>HitSuspiciousTrigger</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,7 +425,7 @@
         <v>200000</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -430,6 +433,14 @@
         <v>200001</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>200002</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now able to update Acquire item task UI for quest
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterKeyEvent.xlsx
+++ b/Assets/Data/Excel/MasterKeyEvent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2CC8C8-F46B-43BF-8EE4-30E4626C5ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFACEE-B080-4735-B2FB-72AE179798DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -42,13 +42,13 @@
     <t>name</t>
   </si>
   <si>
-    <t>ReadBookA</t>
+    <t>None</t>
   </si>
   <si>
-    <t>HitSuspiciousTrigger</t>
+    <t>_200001_ReadBookA</t>
   </si>
   <si>
-    <t>None</t>
+    <t>_200002_HitSuspiciousTrigger</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,7 +425,7 @@
         <v>200000</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -433,7 +433,7 @@
         <v>200001</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,7 +441,7 @@
         <v>200002</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>